<commit_message>
new changes along with new test added
</commit_message>
<xml_diff>
--- a/HybridFramework/TestData/Data.xlsx
+++ b/HybridFramework/TestData/Data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="2" r:id="rId2"/>
-    <sheet name="Leave" sheetId="3" r:id="rId3"/>
+    <sheet name="Leave" sheetId="3" r:id="rId2"/>
+    <sheet name="NewUser" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Admin</t>
   </si>
@@ -24,22 +24,10 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Mukesh500</t>
   </si>
   <si>
-    <t>Mukesh</t>
-  </si>
-  <si>
-    <t>Tools</t>
-  </si>
-  <si>
-    <t>Selenium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place </t>
-  </si>
-  <si>
-    <t>Bangalaore</t>
+    <t>Abcd1234</t>
   </si>
 </sst>
 </file>
@@ -417,48 +405,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -467,4 +413,34 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>